<commit_message>
added admin, password:aninawtechpassw, url:/adminlogin
</commit_message>
<xml_diff>
--- a/SCBAA/2020/NIR.xlsx
+++ b/SCBAA/2020/NIR.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\RESEARCH\2020\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mngx\Desktop\thesis\SCBAA\2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B90D9B4-0526-4A35-B7E8-8CF52070320B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C3F6F5D-02B1-4A45-A2EC-DE355C5B472A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13650" yWindow="240" windowWidth="14625" windowHeight="12540" xr2:uid="{360BF9DE-B15B-43CE-9291-7E05B391F461}"/>
+    <workbookView xWindow="0" yWindow="1830" windowWidth="14880" windowHeight="11070" firstSheet="4" activeTab="8" xr2:uid="{360BF9DE-B15B-43CE-9291-7E05B391F461}"/>
   </bookViews>
   <sheets>
     <sheet name="Bacolod" sheetId="10" r:id="rId1"/>
@@ -36,6 +36,13 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1892,7 +1899,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1EECD59-C1E3-4A87-85F0-D27E48B54FFB}">
   <dimension ref="A1:I112"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -22137,8 +22144,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46E1C0D5-92D8-45B1-805B-D2EA38DB16A5}">
   <dimension ref="A1:I112"/>
   <sheetViews>
-    <sheetView topLeftCell="A91" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E109" activeCellId="29" sqref="E10 E15 E20 E23 E28 E32 E41 E45 E49 E53 E57 E61 E65 E69 E73 E74 E77 E80 E83 E86 E89 E94 E95 E97 E99 E101 E103 E105 E107 E109"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22392,9 +22399,7 @@
         <v>33</v>
       </c>
       <c r="D23" s="8"/>
-      <c r="E23" s="59">
-        <v>0</v>
-      </c>
+      <c r="E23" s="59"/>
     </row>
     <row r="24" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
@@ -22447,9 +22452,7 @@
         <v>38</v>
       </c>
       <c r="D28" s="8"/>
-      <c r="E28" s="63">
-        <v>0</v>
-      </c>
+      <c r="E28" s="63"/>
     </row>
     <row r="29" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>

</xml_diff>